<commit_message>
Romoved two unused variable in SimulinkConfig and removed output from test_field_existence
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/SimulinkConfig.xlsx
+++ b/AD-EYE/TA/Configurations/SimulinkConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAAFCDF-804C-44AE-BC4C-672A0C8AEEEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647E5809-85EC-4F91-AE8D-920560B755D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2904" yWindow="3852" windowWidth="23040" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1368" windowWidth="23040" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>BlockName</t>
   </si>
@@ -82,12 +82,6 @@
   </si>
   <si>
     <t>GoalOrientW</t>
-  </si>
-  <si>
-    <t>GoalTime</t>
-  </si>
-  <si>
-    <t>GoalDistance</t>
   </si>
   <si>
     <t>GnssPoseSimulink</t>
@@ -469,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B18"/>
+      <selection activeCell="A19" sqref="A19:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,7 +623,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -637,7 +631,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -685,7 +679,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -693,7 +687,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>100</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -701,22 +695,6 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed frequencies from the test automation configuration xlsx
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/SimulinkConfig.xlsx
+++ b/AD-EYE/TA/Configurations/SimulinkConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647E5809-85EC-4F91-AE8D-920560B755D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108E7F6D-056E-45C6-9EB2-8A17347E983D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1368" windowWidth="23040" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>BlockName</t>
   </si>
@@ -82,30 +82,6 @@
   </si>
   <si>
     <t>GoalOrientW</t>
-  </si>
-  <si>
-    <t>GnssPoseSimulink</t>
-  </si>
-  <si>
-    <t>PointsRawFloat32</t>
-  </si>
-  <si>
-    <t>ImageRaw</t>
-  </si>
-  <si>
-    <t>ClockFrequency</t>
-  </si>
-  <si>
-    <t>SimulinkState</t>
-  </si>
-  <si>
-    <t>CurrentVelocity</t>
-  </si>
-  <si>
-    <t>PoseOtherCar</t>
-  </si>
-  <si>
-    <t>CurrentPose</t>
   </si>
   <si>
     <t>percent_reflecting_sfc</t>
@@ -463,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD20"/>
+      <selection activeCell="A19" sqref="A19:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,7 +599,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>100</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -631,70 +607,6 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed goal for experiment A
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/SimulinkConfig.xlsx
+++ b/AD-EYE/TA/Configurations/SimulinkConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108E7F6D-056E-45C6-9EB2-8A17347E983D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13281EC6-55C6-4337-84EB-0FA82558D333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1368" windowWidth="23040" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="14724" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD26"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +543,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>220</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -551,7 +551,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>-459</v>
+        <v>-550</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -583,7 +583,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>-0.443</v>
+        <v>-0.55100000000000005</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -591,7 +591,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0.89700000000000002</v>
+        <v>0.83499999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Renamed rain model constants
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/SimulinkConfig.xlsx
+++ b/AD-EYE/TA/Configurations/SimulinkConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13281EC6-55C6-4337-84EB-0FA82558D333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE9A9D2-C04B-4B41-A9A9-4D669BF0DEA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="14724" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,10 +84,10 @@
     <t>GoalOrientW</t>
   </si>
   <si>
-    <t>percent_reflecting_sfc</t>
-  </si>
-  <si>
-    <t>R</t>
+    <t>fi_lidar_rain_reflectivity</t>
+  </si>
+  <si>
+    <t>fi_lidar_rain_intensity</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>